<commit_message>
created a set of user stories
</commit_message>
<xml_diff>
--- a/Design/Planning.xlsx
+++ b/Design/Planning.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Serigraph\Design\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10378FB2-47A9-42AF-8C0E-680AFA4A3C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="UserStories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +25,86 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+  <si>
+    <t>As a student I want to keep track of work on different modules at the same time.</t>
+  </si>
+  <si>
+    <t>As a freelancer I want to track how much time I spend on a given project.</t>
+  </si>
+  <si>
+    <t>As someone that gets distracted easily, I want to set myself short-term objectives as an incentive to tackle my work.</t>
+  </si>
+  <si>
+    <t>As a freelancer I want access to a backlog of tasks I checked off on a given project.</t>
+  </si>
+  <si>
+    <t>As someone with data analysis skills, I want to be able to export data from the system in a .csv format</t>
+  </si>
+  <si>
+    <t>As someone that takes on a lot of self-directed work, I'd like to plan &amp; record sessions of work.</t>
+  </si>
+  <si>
+    <t>As someone with many ongoing projects to keep track of I want a hierarchical tagging/categories system</t>
+  </si>
+  <si>
+    <t>As someone self-employed I want to search back through my sessions of work to find when I was working on certain tasks.</t>
+  </si>
+  <si>
+    <t>As a student that uses colour-encoding to organise my work I want to be able to customise colour of some ui elements/categories.</t>
+  </si>
+  <si>
+    <t>STORY-01</t>
+  </si>
+  <si>
+    <t>STORY-02</t>
+  </si>
+  <si>
+    <t>STORY-03</t>
+  </si>
+  <si>
+    <t>STORY-04</t>
+  </si>
+  <si>
+    <t>STORY-05</t>
+  </si>
+  <si>
+    <t>STORY-06</t>
+  </si>
+  <si>
+    <t>STORY-07</t>
+  </si>
+  <si>
+    <t>STORY-08</t>
+  </si>
+  <si>
+    <t>STORY-09</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +112,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,14 +147,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +458,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62A3FEE1-CF09-42FF-97A7-6AA7FB6BC22D}">
+  <dimension ref="B2:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="15.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="122.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>